<commit_message>
Finished stimulus creation and presentation with PsychoPy.
</commit_message>
<xml_diff>
--- a/input_files/stim-info_gratings-v1.xlsx
+++ b/input_files/stim-info_gratings-v1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burakgur/Documents/GitHub/PyStim/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A646CF9-3D82-2A4D-B35C-7962DCFA978C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEA4A8A5-6FA0-B64D-82D1-3E2E17CEDBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="12300" windowWidth="14580" windowHeight="10940" xr2:uid="{F97281FE-4073-1249-B571-52C9C6825510}"/>
+    <workbookView xWindow="12320" yWindow="460" windowWidth="11280" windowHeight="19080" xr2:uid="{F97281FE-4073-1249-B571-52C9C6825510}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="stim-info_gratings-v1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>stim_type</t>
   </si>
@@ -53,9 +53,6 @@
     <t>gratings-v1</t>
   </si>
   <si>
-    <t>duration_seconds</t>
-  </si>
-  <si>
     <t>direction_deg</t>
   </si>
   <si>
@@ -81,6 +78,15 @@
   </si>
   <si>
     <t>str</t>
+  </si>
+  <si>
+    <t>param7</t>
+  </si>
+  <si>
+    <t>total_dur_sec</t>
+  </si>
+  <si>
+    <t>mean_luminance</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A76F12-96DF-624A-B4F9-C9DA6DA6FEFA}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,68 +466,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>